<commit_message>
Change GroupName to be case-insensitive
</commit_message>
<xml_diff>
--- a/G04_attendance.xlsx
+++ b/G04_attendance.xlsx
@@ -179,7 +179,7 @@
         <v>0.0</v>
       </c>
       <c r="F4" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="G4" t="n">
         <v>0.0</v>
@@ -208,7 +208,7 @@
         <v>0.0</v>
       </c>
       <c r="F5" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="G5" t="n">
         <v>0.0</v>
@@ -237,7 +237,7 @@
         <v>0.0</v>
       </c>
       <c r="F6" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="G6" t="n">
         <v>0.0</v>
@@ -266,7 +266,7 @@
         <v>0.0</v>
       </c>
       <c r="F7" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="G7" t="n">
         <v>0.0</v>
@@ -295,7 +295,7 @@
         <v>0.0</v>
       </c>
       <c r="F8" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="G8" t="n">
         <v>0.0</v>
@@ -324,7 +324,7 @@
         <v>0.0</v>
       </c>
       <c r="F9" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="G9" t="n">
         <v>0.0</v>

</xml_diff>

<commit_message>
Add tests for ExportAttCommandTest and ExportScoreCommandTest
</commit_message>
<xml_diff>
--- a/G04_attendance.xlsx
+++ b/G04_attendance.xlsx
@@ -44,16 +44,10 @@
     <t>4-1</t>
   </si>
   <si>
-    <t>ALICE</t>
-  </si>
-  <si>
-    <t>A0000002U</t>
-  </si>
-  <si>
-    <t>BENNY</t>
-  </si>
-  <si>
-    <t>A0000001U</t>
+    <t>AARON TAN</t>
+  </si>
+  <si>
+    <t>A0123456U</t>
   </si>
   <si>
     <t>BU WEN JIN</t>
@@ -68,16 +62,22 @@
     <t>A0765432U</t>
   </si>
   <si>
-    <t>RYAN LIM</t>
-  </si>
-  <si>
-    <t>A0000000U</t>
-  </si>
-  <si>
-    <t>RYAN TAN</t>
-  </si>
-  <si>
-    <t>A0000004U</t>
+    <t>LIM CHUN YONG</t>
+  </si>
+  <si>
+    <t>A0388443R</t>
+  </si>
+  <si>
+    <t>LIM JIA RUI RYAN</t>
+  </si>
+  <si>
+    <t>A0587314L</t>
+  </si>
+  <si>
+    <t>NEO RUI EN MAYBELLINE</t>
+  </si>
+  <si>
+    <t>A0139345U</t>
   </si>
 </sst>
 </file>

</xml_diff>